<commit_message>
Updating pct code changes
</commit_message>
<xml_diff>
--- a/Sample_Prep_Helper_Template.xlsx
+++ b/Sample_Prep_Helper_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sys_op\methods\Development\AMEX_Template_BD\MVI_Sample_Prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F615802-85F5-4953-B037-ED52750A6055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D34A744-530F-43B8-B33A-02299CC2FBDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1215" yWindow="2475" windowWidth="21600" windowHeight="11295" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MVI_Sample" sheetId="11" r:id="rId1"/>
@@ -455,7 +455,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="694">
   <si>
     <t>Country</t>
   </si>
@@ -2529,13 +2529,16 @@
     <t>ICC - IECC</t>
   </si>
   <si>
-    <t>Update_NA_Cell</t>
-  </si>
-  <si>
     <t>Update_Product</t>
   </si>
   <si>
     <t>Update_PCT_Code</t>
+  </si>
+  <si>
+    <t>NA_Cell_Number</t>
+  </si>
+  <si>
+    <t>Update_NA_Cell_Number</t>
   </si>
 </sst>
 </file>
@@ -2950,14 +2953,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3197,12 +3201,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="4" xr:uid="{FB8B6281-A8C0-447B-9B77-C69B201BCCA9}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{12D21FF4-3EA1-4D98-B8E6-4E381D0403C9}"/>
+    <cellStyle name="Normal 4" xfId="5" xr:uid="{3BE77019-FFC4-493F-BCD4-5600AF532C12}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
@@ -23641,7 +23652,7 @@
   </sheetPr>
   <dimension ref="A1:Z294"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="84" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="84" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="7" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="F16" sqref="F16"/>
     </sheetView>
@@ -48604,326 +48615,38 @@
       <c r="Z16"/>
       <c r="AD16"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="C17"/>
-      <c r="G17"/>
-      <c r="K17"/>
-      <c r="O17"/>
-      <c r="V17"/>
-      <c r="Z17"/>
-      <c r="AD17"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="C18"/>
-      <c r="G18"/>
-      <c r="K18"/>
-      <c r="O18"/>
-      <c r="V18"/>
-      <c r="Z18"/>
-      <c r="AD18"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="C19"/>
-      <c r="G19"/>
-      <c r="K19"/>
-      <c r="O19"/>
-      <c r="V19"/>
-      <c r="Z19"/>
-      <c r="AD19"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="C20"/>
-      <c r="G20"/>
-      <c r="K20"/>
-      <c r="O20"/>
-      <c r="V20"/>
-      <c r="Z20"/>
-      <c r="AD20"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="C21"/>
-      <c r="G21"/>
-      <c r="K21"/>
-      <c r="O21"/>
-      <c r="V21"/>
-      <c r="Z21"/>
-      <c r="AD21"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="C22"/>
-      <c r="G22"/>
-      <c r="K22"/>
-      <c r="O22"/>
-      <c r="V22"/>
-      <c r="Z22"/>
-      <c r="AD22"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="C23"/>
-      <c r="G23"/>
-      <c r="K23"/>
-      <c r="O23"/>
-      <c r="V23"/>
-      <c r="Z23"/>
-      <c r="AD23"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="C24"/>
-      <c r="G24"/>
-      <c r="K24"/>
-      <c r="O24"/>
-      <c r="V24"/>
-      <c r="Z24"/>
-      <c r="AD24"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="C25"/>
-      <c r="G25"/>
-      <c r="K25"/>
-      <c r="O25"/>
-      <c r="V25"/>
-      <c r="Z25"/>
-      <c r="AD25"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="C26"/>
-      <c r="G26"/>
-      <c r="K26"/>
-      <c r="O26"/>
-      <c r="V26"/>
-      <c r="Z26"/>
-      <c r="AD26"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-      <c r="C27"/>
-      <c r="G27"/>
-      <c r="K27"/>
-      <c r="O27"/>
-      <c r="V27"/>
-      <c r="Z27"/>
-      <c r="AD27"/>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A28"/>
-      <c r="C28"/>
-      <c r="G28"/>
-      <c r="K28"/>
-      <c r="O28"/>
-      <c r="V28"/>
-      <c r="Z28"/>
-      <c r="AD28"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A29"/>
-      <c r="C29"/>
-      <c r="G29"/>
-      <c r="K29"/>
-      <c r="O29"/>
-      <c r="V29"/>
-      <c r="Z29"/>
-      <c r="AD29"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A30"/>
-      <c r="C30"/>
-      <c r="G30"/>
-      <c r="K30"/>
-      <c r="O30"/>
-      <c r="V30"/>
-      <c r="Z30"/>
-      <c r="AD30"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-      <c r="C31"/>
-      <c r="G31"/>
-      <c r="K31"/>
-      <c r="O31"/>
-      <c r="V31"/>
-      <c r="Z31"/>
-      <c r="AD31"/>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A32"/>
-      <c r="C32"/>
-      <c r="G32"/>
-      <c r="K32"/>
-      <c r="O32"/>
-      <c r="V32"/>
-      <c r="Z32"/>
-      <c r="AD32"/>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-      <c r="C33"/>
-      <c r="G33"/>
-      <c r="K33"/>
-      <c r="O33"/>
-      <c r="V33"/>
-      <c r="Z33"/>
-      <c r="AD33"/>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-      <c r="C34"/>
-      <c r="G34"/>
-      <c r="K34"/>
-      <c r="O34"/>
-      <c r="V34"/>
-      <c r="Z34"/>
-      <c r="AD34"/>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A35"/>
-      <c r="C35"/>
-      <c r="G35"/>
-      <c r="K35"/>
-      <c r="O35"/>
-      <c r="V35"/>
-      <c r="Z35"/>
-      <c r="AD35"/>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-      <c r="C36"/>
-      <c r="G36"/>
-      <c r="K36"/>
-      <c r="O36"/>
-      <c r="V36"/>
-      <c r="Z36"/>
-      <c r="AD36"/>
-    </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-      <c r="C37"/>
-      <c r="G37"/>
-      <c r="K37"/>
-      <c r="O37"/>
-      <c r="V37"/>
-      <c r="Z37"/>
-      <c r="AD37"/>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A38"/>
-      <c r="C38"/>
-      <c r="G38"/>
-      <c r="K38"/>
-      <c r="O38"/>
-      <c r="V38"/>
-      <c r="Z38"/>
-      <c r="AD38"/>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-      <c r="C39"/>
-      <c r="G39"/>
-      <c r="K39"/>
-      <c r="O39"/>
-      <c r="V39"/>
-      <c r="Z39"/>
-      <c r="AD39"/>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-      <c r="C40"/>
-      <c r="G40"/>
-      <c r="K40"/>
-      <c r="O40"/>
-      <c r="V40"/>
-      <c r="Z40"/>
-      <c r="AD40"/>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-      <c r="C41"/>
-      <c r="G41"/>
-      <c r="K41"/>
-      <c r="O41"/>
-      <c r="V41"/>
-      <c r="Z41"/>
-      <c r="AD41"/>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A42"/>
-      <c r="C42"/>
-      <c r="G42"/>
-      <c r="K42"/>
-      <c r="O42"/>
-      <c r="V42"/>
-      <c r="Z42"/>
-      <c r="AD42"/>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A43"/>
-      <c r="C43"/>
-      <c r="G43"/>
-      <c r="K43"/>
-      <c r="O43"/>
-      <c r="V43"/>
-      <c r="Z43"/>
-      <c r="AD43"/>
-    </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A44"/>
-      <c r="C44"/>
-      <c r="G44"/>
-      <c r="K44"/>
-      <c r="O44"/>
-      <c r="V44"/>
-      <c r="Z44"/>
-      <c r="AD44"/>
-    </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A45"/>
-      <c r="C45"/>
-      <c r="G45"/>
-      <c r="K45"/>
-      <c r="O45"/>
-      <c r="V45"/>
-      <c r="Z45"/>
-      <c r="AD45"/>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A46"/>
-      <c r="C46"/>
-      <c r="G46"/>
-      <c r="K46"/>
-      <c r="O46"/>
-      <c r="V46"/>
-      <c r="Z46"/>
-      <c r="AD46"/>
-    </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A47"/>
-      <c r="C47"/>
-      <c r="G47"/>
-      <c r="K47"/>
-      <c r="O47"/>
-      <c r="V47"/>
-      <c r="Z47"/>
-      <c r="AD47"/>
-    </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A48"/>
-      <c r="C48"/>
-      <c r="G48"/>
-      <c r="K48"/>
-      <c r="O48"/>
-      <c r="V48"/>
-      <c r="Z48"/>
-      <c r="AD48"/>
-    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -51975,52 +51698,48 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41731C0D-7C85-4CD0-AAB2-C08CD9D76422}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="95" t="s">
         <v>163</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="F1" s="96" t="s">
+        <v>693</v>
+      </c>
+      <c r="G1" s="96" t="s">
         <v>690</v>
       </c>
-      <c r="H1" s="81" t="s">
+      <c r="H1" s="96" t="s">
         <v>691</v>
-      </c>
-      <c r="I1" s="81" t="s">
-        <v>692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>